<commit_message>
new excel sheets added to improve performance.
</commit_message>
<xml_diff>
--- a/matlabApp.xlsx
+++ b/matlabApp.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Desktop/matlabApp/tankDeneyMatlab/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Desktop/pullProject/tankApp/tankApp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C864F70-F324-254A-BDF3-C39A114941C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F598FC33-4965-104F-9253-248B723CF7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2660" yWindow="500" windowWidth="22940" windowHeight="13560" xr2:uid="{A33F9FD5-AFDC-A941-8D27-8AB5E1F101F0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="198">
   <si>
     <t>40 lpm - hole 1 - diameter 6</t>
   </si>
@@ -496,6 +496,138 @@
   </si>
   <si>
     <t>120 lpm - hole 6 + 7 - diameter 12</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 6 + 7 - diameter 12 (Boğaza Bağlı)</t>
+  </si>
+  <si>
+    <t>23.08.2021</t>
+  </si>
+  <si>
+    <t>17:12:41</t>
+  </si>
+  <si>
+    <t>40 lpm - hole 6 + 7 - diameter 12 (Boğaza Bağlı)</t>
+  </si>
+  <si>
+    <t>08:41:49</t>
+  </si>
+  <si>
+    <t>24.08.2021</t>
+  </si>
+  <si>
+    <t>40 lpm - hole 4 + 5 - diameter 12 (Boğaza Bağlı)</t>
+  </si>
+  <si>
+    <t>40 lpm - hole 5 + 7 - diameter 12 (Boğaza Bağlı)</t>
+  </si>
+  <si>
+    <t>08:57:36</t>
+  </si>
+  <si>
+    <t>40 lpm - hole 5 + 6 - diameter 12 (Boğaza Bağlı)</t>
+  </si>
+  <si>
+    <t>09:16:58</t>
+  </si>
+  <si>
+    <t>40 lpm - hole 3 + 7 - diameter 12 (Boğaza Bağlı)</t>
+  </si>
+  <si>
+    <t>09:38:16</t>
+  </si>
+  <si>
+    <t>80 lpm - hole 6 + 7 - diameter 12 (Boğaza Bağlı)</t>
+  </si>
+  <si>
+    <t>25.08.2021</t>
+  </si>
+  <si>
+    <t>08:27:03</t>
+  </si>
+  <si>
+    <t>80 lpm - hole 4 + 5 - diameter 12 (Boğaza Bağlı)</t>
+  </si>
+  <si>
+    <t>08:42:45</t>
+  </si>
+  <si>
+    <t>80 lpm - hole 5 + 7 - diameter 12 (Boğaza Bağlı)</t>
+  </si>
+  <si>
+    <t>09:05:28</t>
+  </si>
+  <si>
+    <t>07:49:04</t>
+  </si>
+  <si>
+    <t>27.08.2021</t>
+  </si>
+  <si>
+    <t>80 lpm - hole 5 + 6 - diameter 12 (Boğaza Bağlı)</t>
+  </si>
+  <si>
+    <t>80 lpm - hole 3 + 7 - diameter 12 (Boğaza Bağlı)</t>
+  </si>
+  <si>
+    <t>08:05:59</t>
+  </si>
+  <si>
+    <t>09:51:15</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 4 + 5 - diameter 12 (Boğaza Bağlı)</t>
+  </si>
+  <si>
+    <t>10:29:22</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 5 + 7 - diameter 12 (Boğaza Bağlı)</t>
+  </si>
+  <si>
+    <t>10:48:07</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 5 + 6 - diameter 12 (Boğaza Bağlı)</t>
+  </si>
+  <si>
+    <t>11:07:14</t>
+  </si>
+  <si>
+    <t>11:36:18</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 3 + 7 - diameter 12 (Boğaza Bağlı)</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 1 + 2 - diameter 12 (Boğaza Bağlı)</t>
+  </si>
+  <si>
+    <t>14:07:43</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 1 + 3 - diameter 12 (Boğaza Bağlı)</t>
+  </si>
+  <si>
+    <t>14:24:27</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 1 + 4 - diameter 12 (Boğaza Bağlı)</t>
+  </si>
+  <si>
+    <t>14:45:06</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 2 + 3 - diameter 12 (Boğaza Bağlı)</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 2 + 4 - diameter 12 (Boğaza Bağlı)</t>
+  </si>
+  <si>
+    <t>16:08:54</t>
+  </si>
+  <si>
+    <t>16:25:49</t>
   </si>
 </sst>
 </file>
@@ -858,15 +990,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69899DAB-4772-1343-B8D3-97A5E67EDB8D}">
-  <dimension ref="A1:C73"/>
+  <dimension ref="A1:C93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
-      <selection activeCell="F56" sqref="F56"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="99" workbookViewId="0">
+      <selection activeCell="F84" sqref="F84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" customWidth="1"/>
+    <col min="1" max="1" width="42.1640625" customWidth="1"/>
     <col min="2" max="3" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -1673,6 +1805,226 @@
         <v>140</v>
       </c>
     </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>157</v>
+      </c>
+      <c r="B74" t="s">
+        <v>156</v>
+      </c>
+      <c r="C74" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
+        <v>160</v>
+      </c>
+      <c r="B75" t="s">
+        <v>158</v>
+      </c>
+      <c r="C75" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A76" t="s">
+        <v>161</v>
+      </c>
+      <c r="B76" t="s">
+        <v>162</v>
+      </c>
+      <c r="C76" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A77" t="s">
+        <v>163</v>
+      </c>
+      <c r="B77" t="s">
+        <v>164</v>
+      </c>
+      <c r="C77" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A78" t="s">
+        <v>165</v>
+      </c>
+      <c r="B78" t="s">
+        <v>166</v>
+      </c>
+      <c r="C78" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A79" t="s">
+        <v>167</v>
+      </c>
+      <c r="B79" t="s">
+        <v>169</v>
+      </c>
+      <c r="C79" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A80" t="s">
+        <v>170</v>
+      </c>
+      <c r="B80" t="s">
+        <v>171</v>
+      </c>
+      <c r="C80" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A81" t="s">
+        <v>172</v>
+      </c>
+      <c r="B81" t="s">
+        <v>173</v>
+      </c>
+      <c r="C81" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A82" t="s">
+        <v>176</v>
+      </c>
+      <c r="B82" t="s">
+        <v>174</v>
+      </c>
+      <c r="C82" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A83" t="s">
+        <v>177</v>
+      </c>
+      <c r="B83" t="s">
+        <v>178</v>
+      </c>
+      <c r="C83" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A84" t="s">
+        <v>154</v>
+      </c>
+      <c r="B84" t="s">
+        <v>179</v>
+      </c>
+      <c r="C84" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A85" t="s">
+        <v>180</v>
+      </c>
+      <c r="B85" t="s">
+        <v>181</v>
+      </c>
+      <c r="C85" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A86" t="s">
+        <v>182</v>
+      </c>
+      <c r="B86" t="s">
+        <v>183</v>
+      </c>
+      <c r="C86" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A87" t="s">
+        <v>184</v>
+      </c>
+      <c r="B87" t="s">
+        <v>185</v>
+      </c>
+      <c r="C87" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A88" t="s">
+        <v>187</v>
+      </c>
+      <c r="B88" t="s">
+        <v>186</v>
+      </c>
+      <c r="C88" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A89" t="s">
+        <v>188</v>
+      </c>
+      <c r="B89" t="s">
+        <v>189</v>
+      </c>
+      <c r="C89" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A90" t="s">
+        <v>190</v>
+      </c>
+      <c r="B90" t="s">
+        <v>191</v>
+      </c>
+      <c r="C90" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A91" t="s">
+        <v>192</v>
+      </c>
+      <c r="B91" t="s">
+        <v>193</v>
+      </c>
+      <c r="C91" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A92" t="s">
+        <v>194</v>
+      </c>
+      <c r="B92" t="s">
+        <v>196</v>
+      </c>
+      <c r="C92" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A93" t="s">
+        <v>195</v>
+      </c>
+      <c r="B93" t="s">
+        <v>197</v>
+      </c>
+      <c r="C93" t="s">
+        <v>175</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new files are added
</commit_message>
<xml_diff>
--- a/matlabApp.xlsx
+++ b/matlabApp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Desktop/pullProject/tankApp/tankApp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F598FC33-4965-104F-9253-248B723CF7B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA4D372-FB3A-A24B-97C0-C0CDE572B556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2660" yWindow="500" windowWidth="22940" windowHeight="13560" xr2:uid="{A33F9FD5-AFDC-A941-8D27-8AB5E1F101F0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="204">
   <si>
     <t>40 lpm - hole 1 - diameter 6</t>
   </si>
@@ -628,6 +628,24 @@
   </si>
   <si>
     <t>16:25:49</t>
+  </si>
+  <si>
+    <t>09:51:34</t>
+  </si>
+  <si>
+    <t>31.08.2021</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 1 + 2 - diameter 12 (Aparatsız)</t>
+  </si>
+  <si>
+    <t>10:45:14</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 2 + 3 - diameter 12 (Aparatsız)</t>
+  </si>
+  <si>
+    <t>11:04:34</t>
   </si>
 </sst>
 </file>
@@ -990,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69899DAB-4772-1343-B8D3-97A5E67EDB8D}">
-  <dimension ref="A1:C93"/>
+  <dimension ref="A1:C96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="99" workbookViewId="0">
-      <selection activeCell="F84" sqref="F84"/>
+    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="99" workbookViewId="0">
+      <selection activeCell="E87" sqref="E87"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2025,6 +2043,39 @@
         <v>175</v>
       </c>
     </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A94" t="s">
+        <v>200</v>
+      </c>
+      <c r="B94" t="s">
+        <v>198</v>
+      </c>
+      <c r="C94" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A95" t="s">
+        <v>202</v>
+      </c>
+      <c r="B95" t="s">
+        <v>201</v>
+      </c>
+      <c r="C95" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A96" t="s">
+        <v>202</v>
+      </c>
+      <c r="B96" t="s">
+        <v>203</v>
+      </c>
+      <c r="C96" t="s">
+        <v>199</v>
+      </c>
+    </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
new data files are added
</commit_message>
<xml_diff>
--- a/matlabApp.xlsx
+++ b/matlabApp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/macbook/Desktop/pullProject/tankApp/tankApp/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EA4D372-FB3A-A24B-97C0-C0CDE572B556}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EC0EACC-5814-EF4F-B93B-2BEF28006552}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2660" yWindow="500" windowWidth="22940" windowHeight="13560" xr2:uid="{A33F9FD5-AFDC-A941-8D27-8AB5E1F101F0}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="244">
   <si>
     <t>40 lpm - hole 1 - diameter 6</t>
   </si>
@@ -646,6 +646,126 @@
   </si>
   <si>
     <t>11:04:34</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 2 + 4 - diameter 12 (Aparatsız)</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 3 + 4 - diameter 12 (Aparatsız)</t>
+  </si>
+  <si>
+    <t>12:12:31</t>
+  </si>
+  <si>
+    <t>12:26:08</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 3 + 5 - diameter 12 (Aparatsız)</t>
+  </si>
+  <si>
+    <t>12:37:36</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 3 + 6 - diameter 12 (Aparatsız)</t>
+  </si>
+  <si>
+    <t>13:41:35</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 3 + 7 - diameter 12 (Aparatsız)</t>
+  </si>
+  <si>
+    <t>13:52:39</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 4 + 5 - diameter 12 (Aparatsız)</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 4 + 6 - diameter 12 (Aparatsız)</t>
+  </si>
+  <si>
+    <t>14:03:08</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 4 + 7 - diameter 12 (Aparatsız)</t>
+  </si>
+  <si>
+    <t>14:21:07</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 5 + 6 - diameter 12 (Aparatsız)</t>
+  </si>
+  <si>
+    <t>14:41:10</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 5 + 7 - diameter 12 (Aparatsız)</t>
+  </si>
+  <si>
+    <t>14:51:05</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 6 + 7 - diameter 12 (Aparatsız)</t>
+  </si>
+  <si>
+    <t>15:19:29</t>
+  </si>
+  <si>
+    <t>10:42:54</t>
+  </si>
+  <si>
+    <t>1.09.2021</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 1 + 2 + 3 - diameter 12 (Aparatsız)</t>
+  </si>
+  <si>
+    <t>11:48:46</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 1 + 2 + 4 - diameter 12 (Aparatsız)</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 1 + 2 + 5 - diameter 12 (Aparatsız)</t>
+  </si>
+  <si>
+    <t>12:01:50</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 2 + 3 + 4 - diameter 12 (Aparatsız)</t>
+  </si>
+  <si>
+    <t>12:32:03</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 2 + 3 + 5 - diameter 12 (Aparatsız)</t>
+  </si>
+  <si>
+    <t>13:44:38</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 2 + 3 + 6 - diameter 12 (Aparatsız)</t>
+  </si>
+  <si>
+    <t>14:07:15</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 2 + 3 + 7 - diameter 12 (Aparatsız)</t>
+  </si>
+  <si>
+    <t>15:50:34</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 2 + 4 + 5 - diameter 12 (Aparatsız)</t>
+  </si>
+  <si>
+    <t>16:26:28</t>
+  </si>
+  <si>
+    <t>120 lpm - hole 3 + 4 + 5 - diameter 12 (Aparatsız)</t>
+  </si>
+  <si>
+    <t>16:52:13</t>
   </si>
 </sst>
 </file>
@@ -689,9 +809,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1008,10 +1131,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69899DAB-4772-1343-B8D3-97A5E67EDB8D}">
-  <dimension ref="A1:C96"/>
+  <dimension ref="A1:C115"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A74" zoomScale="99" workbookViewId="0">
-      <selection activeCell="E87" sqref="E87"/>
+    <sheetView tabSelected="1" topLeftCell="A92" zoomScale="99" workbookViewId="0">
+      <selection activeCell="F112" sqref="F112"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2067,13 +2190,222 @@
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
-        <v>202</v>
+        <v>204</v>
       </c>
       <c r="B96" t="s">
         <v>203</v>
       </c>
       <c r="C96" t="s">
         <v>199</v>
+      </c>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A97" t="s">
+        <v>205</v>
+      </c>
+      <c r="B97" t="s">
+        <v>206</v>
+      </c>
+      <c r="C97" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>208</v>
+      </c>
+      <c r="B98" t="s">
+        <v>207</v>
+      </c>
+      <c r="C98" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>210</v>
+      </c>
+      <c r="B99" t="s">
+        <v>209</v>
+      </c>
+      <c r="C99" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
+        <v>212</v>
+      </c>
+      <c r="B100" t="s">
+        <v>211</v>
+      </c>
+      <c r="C100" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A101" t="s">
+        <v>214</v>
+      </c>
+      <c r="B101" t="s">
+        <v>213</v>
+      </c>
+      <c r="C101" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A102" t="s">
+        <v>215</v>
+      </c>
+      <c r="B102" t="s">
+        <v>216</v>
+      </c>
+      <c r="C102" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A103" t="s">
+        <v>217</v>
+      </c>
+      <c r="B103" t="s">
+        <v>218</v>
+      </c>
+      <c r="C103" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A104" t="s">
+        <v>219</v>
+      </c>
+      <c r="B104" t="s">
+        <v>220</v>
+      </c>
+      <c r="C104" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A105" t="s">
+        <v>221</v>
+      </c>
+      <c r="B105" t="s">
+        <v>222</v>
+      </c>
+      <c r="C105" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A106" t="s">
+        <v>223</v>
+      </c>
+      <c r="B106" t="s">
+        <v>224</v>
+      </c>
+      <c r="C106" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A107" t="s">
+        <v>227</v>
+      </c>
+      <c r="B107" t="s">
+        <v>225</v>
+      </c>
+      <c r="C107" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>229</v>
+      </c>
+      <c r="B108" t="s">
+        <v>228</v>
+      </c>
+      <c r="C108" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>230</v>
+      </c>
+      <c r="B109" t="s">
+        <v>231</v>
+      </c>
+      <c r="C109" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>232</v>
+      </c>
+      <c r="B110" t="s">
+        <v>233</v>
+      </c>
+      <c r="C110" s="2">
+        <v>44440</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
+        <v>234</v>
+      </c>
+      <c r="B111" t="s">
+        <v>235</v>
+      </c>
+      <c r="C111" s="2">
+        <v>44440</v>
+      </c>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A112" t="s">
+        <v>236</v>
+      </c>
+      <c r="B112" t="s">
+        <v>237</v>
+      </c>
+      <c r="C112" s="2">
+        <v>44440</v>
+      </c>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A113" t="s">
+        <v>238</v>
+      </c>
+      <c r="B113" t="s">
+        <v>239</v>
+      </c>
+      <c r="C113" s="2">
+        <v>44440</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>240</v>
+      </c>
+      <c r="B114" t="s">
+        <v>241</v>
+      </c>
+      <c r="C114" s="2">
+        <v>44440</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>242</v>
+      </c>
+      <c r="B115" t="s">
+        <v>243</v>
+      </c>
+      <c r="C115" s="2">
+        <v>44440</v>
       </c>
     </row>
   </sheetData>

</xml_diff>